<commit_message>
included the first 400 ppm point in SS curves
</commit_message>
<xml_diff>
--- a/1_Raw_data/2022-08-11-0949_walkup_aci_clean.xlsx
+++ b/1_Raw_data/2022-08-11-0949_walkup_aci_clean.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmel\Desktop\DAT_proj\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmel\Desktop\DAT_proj\1_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCA74E2-71E9-4F7E-914F-D9F87A5452F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029CFFB7-1704-477F-96B4-E0B8FD4D4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,17 @@
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
     <sheet name="Remarks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="424">
   <si>
     <t>File opened</t>
   </si>
@@ -1303,9 +1306,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>exclude</t>
   </si>
 </sst>
 </file>
@@ -1361,9 +1361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1401,9 +1401,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1436,26 +1436,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1488,26 +1471,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1684,7 +1650,7 @@
   <dimension ref="A2:IN27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="HR9" workbookViewId="0">
-      <selection activeCell="IN18" sqref="IN18"/>
+      <selection activeCell="IN17" sqref="IN17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4830,7 +4796,7 @@
         <v>100.37</v>
       </c>
       <c r="IN17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="1:248" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
removed the first point from the SS curves again
</commit_message>
<xml_diff>
--- a/1_Raw_data/2022-08-11-0949_walkup_aci_clean.xlsx
+++ b/1_Raw_data/2022-08-11-0949_walkup_aci_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmel\Desktop\DAT_proj\1_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029CFFB7-1704-477F-96B4-E0B8FD4D4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EA8D7D-F097-4814-B338-C5D1E934CC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="425">
   <si>
     <t>File opened</t>
   </si>
@@ -1306,6 +1306,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>exclude</t>
   </si>
 </sst>
 </file>
@@ -1649,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:IN27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HR9" workbookViewId="0">
-      <selection activeCell="IN17" sqref="IN17"/>
+    <sheetView tabSelected="1" topLeftCell="HY2" workbookViewId="0">
+      <selection activeCell="IN18" sqref="IN18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4796,7 +4799,7 @@
         <v>100.37</v>
       </c>
       <c r="IN17" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:248" x14ac:dyDescent="0.3">

</xml_diff>